<commit_message>
Added DOTA and rotated mnist results
</commit_message>
<xml_diff>
--- a/results/results_DOTAv1.0.xlsx
+++ b/results/results_DOTAv1.0.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\school\e2cnn_experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F36A93-D105-40FE-BE39-59441F4E110F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B63DF0-A6AB-4CA4-9F3C-427357CC0F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="22950" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4275" yWindow="735" windowWidth="22950" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="model_DOTAv1.0 - Copy" sheetId="1" r:id="rId1"/>
+    <sheet name="model_DOTAv1.0" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -684,7 +684,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$B$1</c:f>
+              <c:f>model_DOTAv1.0!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -707,7 +707,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$B$2:$B$101</c:f>
+              <c:f>model_DOTAv1.0!$B$2:$B$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1026,7 +1026,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$D$1</c:f>
+              <c:f>model_DOTAv1.0!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1050,7 +1050,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$D$2:$D$101</c:f>
+              <c:f>model_DOTAv1.0!$D$2:$D$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1369,7 +1369,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$F$1</c:f>
+              <c:f>model_DOTAv1.0!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1392,7 +1392,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$F$2:$F$101</c:f>
+              <c:f>model_DOTAv1.0!$F$2:$F$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1440,6 +1440,261 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>87.9911993450675</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>88.782933540000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>89.847306529999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>89.927496329999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90.728388469999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>90.647668390000007</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>91.001683499999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>91.982758619999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>91.995192309999993</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>92.386541469999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>92.496177369999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>92.795216740000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>92.918535129999995</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>93.512705530000005</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>93.744394619999994</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>93.7593423</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>94.129297458893802</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>94.222720478325797</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>94.155455904334801</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>94.816890881913295</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>94.783258594917697</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>94.633781763826605</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>94.947683109118003</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>95.411061285500693</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>95.526905829596402</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>95.313901345291399</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>95.642750373691996</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>95.766068759342303</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>95.620328849028397</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>96.079970104633702</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>95.874439461883398</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>95.769805680119504</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>96.147234678624798</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>96.177130044842997</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>96.259342301943093</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>96.296711509715905</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>96.263079222720407</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>96.677877428998499</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>96.513452914798194</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>96.603139013452903</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>96.6704035874439</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>96.603139013452903</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>96.875934230194304</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>96.860986547085204</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>96.842301943198805</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>97.010463378176297</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>96.920777279521602</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>96.875934230194304</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>97.320627802690495</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>97.096412556053806</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>97.2346786248131</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>97.275784753363197</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>97.115097159940206</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>97.320627802690495</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>97.399103139013405</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>97.305680119581396</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>97.331838565022395</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>97.552316890881897</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>97.212257100149401</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>97.690582959641205</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>97.612107623318394</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>97.623318385650194</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>97.634529147981993</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>97.619581464872894</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>97.713004484304903</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>97.675635276532105</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>97.754110612855001</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>97.832585949177798</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>97.776532137518601</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>97.862481315396096</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>97.713004484304903</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>97.813901345291399</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>97.769058295964101</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>98.090433482810099</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>98.015695067264502</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>97.754110612855001</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>98.041853512705501</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>97.836322869955097</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>98.049327354260001</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>97.888639760836995</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>98.127802690582897</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>98.011958146487302</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>98.127802690582897</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>97.963378176382605</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>98.307174887892302</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>98.120328849028397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1456,7 +1711,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$H$1</c:f>
+              <c:f>model_DOTAv1.0!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1480,7 +1735,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$H$2:$H$101</c:f>
+              <c:f>model_DOTAv1.0!$H$2:$H$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1528,6 +1783,261 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>79.873821408763106</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80.466583470000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>81.444120909999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>79.586106490000006</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>80.983083750000006</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>80.65030505</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>81.468386019999997</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>82.882695510000005</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>81.880892959999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>82.182473659999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>82.189406539999993</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>81.953688299999996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>83.187742650000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>82.581114810000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>83.569051580000007</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>82.425124789999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>83.4061286744315</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>83.270937326677696</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>82.321131447587305</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>82.556849694952803</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>83.184276206322707</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>83.901830282861894</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>82.997088186355995</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>83.191209095951194</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>83.4303937881309</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>83.385330005546294</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>83.641846921796997</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>83.777038269550701</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>83.811702717692697</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>83.985024958402605</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>84.362867443150293</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>83.704242928452501</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>83.666112035496397</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>84.023155851358794</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>83.856766500277303</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>84.758042151968894</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>83.035219079312199</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>84.463394342762001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>83.607182473655001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>84.300471436494703</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>84.737243483083702</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>84.380199667221305</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>84.654048807542907</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>84.258874098724306</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>84.487659456461401</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>84.075152523571802</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>84.120216306156394</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>84.383666112035499</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>84.723377703826898</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>84.179145867997704</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>84.785773710482502</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>84.543122573488603</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>83.835967831392097</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>84.737243483083702</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>84.283139212423706</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>84.432196339434199</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>84.678313921242307</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>84.848169717138106</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>84.206877426511298</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>84.657515252357101</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>84.491125901275595</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>84.154880754298304</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>85.132418191902303</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>84.168746533555094</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>84.719911259012704</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>84.470327232390403</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>84.622850804215204</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>85.011092623405403</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>84.910565723793596</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84.771907931225698</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84.570854132002196</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>84.078618968385996</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>84.751109262340506</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>84.6817803660565</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>84.841236827509704</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>84.130615640599004</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>84.657515252357101</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>84.751109262340506</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>84.813505268996096</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>84.355934553521905</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>85.461730449251206</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>84.269273433166902</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>84.7060454797559</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>84.394065446478095</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>84.789240155296696</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>84.473793677204597</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1836,7 +2346,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$C$1</c:f>
+              <c:f>model_DOTAv1.0!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1859,7 +2369,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$C$2:$C$101</c:f>
+              <c:f>model_DOTAv1.0!$C$2:$C$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -2178,7 +2688,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$E$1</c:f>
+              <c:f>model_DOTAv1.0!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2202,7 +2712,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$E$2:$E$101</c:f>
+              <c:f>model_DOTAv1.0!$E$2:$E$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -2521,7 +3031,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$G$1</c:f>
+              <c:f>model_DOTAv1.0!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2544,7 +3054,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$G$2:$G$101</c:f>
+              <c:f>model_DOTAv1.0!$G$2:$G$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -2592,6 +3102,261 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>982.40521240234295</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>951.46722409999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>897.05731200000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>915.60192870000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>870.22143549999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>880.37701419999996</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>866.34460449999995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>813.19372559999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>817.13684079999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>784.27227779999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>782.26184079999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>778.23474120000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>756.52508539999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>698.95031740000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>671.10034180000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>662.51641849999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>621.66497802734295</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>599.49212646484295</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>607.22607421875</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>547.78076171875</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>555.03466796875</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>561.5966796875</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>516.11614990234295</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>485.562255859375</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>462.63967895507801</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>484.35003662109301</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>452.96243286132801</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>449.43307495117102</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>457.09313964843699</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>402.15637207031199</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>426.25921630859301</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>418.59878540039</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>398.88113403320301</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>387.63302612304602</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>377.62649536132801</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>379.46697998046801</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>375.00848388671801</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>358.18258666992102</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>360.98452758789</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>344.29818725585898</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>332.98245239257801</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>340.19583129882801</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>325.78228759765602</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>322.43563842773398</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>316.82492065429602</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>318.410552978515</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>319.89273071289</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>321.06829833984301</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>285.01052856445301</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>292.65679931640602</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>284.40121459960898</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>279.76776123046801</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>282.517822265625</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>270.57080078125</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>270.22692871093699</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>274.60610961914</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>269.64254760742102</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>254.59205627441401</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>277.28131103515602</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>241.49928283691401</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>234.65965270996</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>243.79116821289</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>235.63536071777301</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>250.30729675292901</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>237.21122741699199</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>239.29904174804599</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>232.43489074707</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>215.68127441406199</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>228.06394958496</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>214.60850524902301</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>225.80044555664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>225.41110229492099</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>226.17283630371</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>203.05740356445301</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>195.89602661132801</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>220.155014038085</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>204.89091491699199</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>226.47520446777301</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>200.84881591796801</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>212.31690979003901</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>187.22636413574199</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>196.883056640625</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>188.84878540039</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>198.51150512695301</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>179.83720397949199</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>182.00682067871</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2608,7 +3373,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$I$1</c:f>
+              <c:f>model_DOTAv1.0!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2632,7 +3397,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'model_DOTAv1.0 - Copy'!$I$2:$I$101</c:f>
+              <c:f>model_DOTAv1.0!$I$2:$I$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -2680,6 +3445,261 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>2302.2021484375</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2313.7700199999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2150.6447750000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2374.544922</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2233.4907229999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2305.0996089999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2179.7448730000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1968.4338379999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2098.0234380000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2159.5668949999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2111.4914549999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2148.7602539999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2022.4293210000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2077.8610840000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2001.299927</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2162.5109859999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2014.80822753906</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2070.4775390625</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2241.36645507812</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2177.02709960937</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2107.146484375</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2017.041015625</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2129.21508789062</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2137.876953125</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2122.11791992187</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2159.12158203125</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2126.5498046875</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2097.83569335937</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2172.41015625</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2103.43701171875</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2053.2470703125</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2182.51147460937</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2200.10913085937</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2190.8212890625</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2133.96240234375</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2087.52758789062</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2222.9765625</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2095.80126953125</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2284.13208007812</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2185.57568359375</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2097.6953125</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2132.11010742187</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2158.64453125</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2132.5341796875</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2219.94750976562</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2244.015625</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2258.71215820312</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2192.31811523437</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2164.91381835937</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2202.30493164062</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2146.08911132812</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2200.2900390625</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2300.919921875</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2239.9287109375</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2204.99658203125</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2260.31762695312</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2241.73999023437</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2228.33422851562</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2281.2568359375</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2295.232421875</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2313.78247070312</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2349.74487304687</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2228.49487304687</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2352.32397460937</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2246.421875</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2419.63891601562</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2315.99145507812</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2316.21166992187</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2281.05859375</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2259.4287109375</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2345.05029296875</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2380.4287109375</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2321.81274414062</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2342.87524414062</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2310.34594726562</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2487.59252929687</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2351.63696289062</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2333.14404296875</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2330.47387695312</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2412.3115234375</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2258.31420898437</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2458.80029296875</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2329.93603515625</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2386.41918945312</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2407.47583007812</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2493.00463867187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4849,7 +5869,7 @@
         <v>2302.2021484375</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4865,8 +5885,20 @@
       <c r="E17">
         <v>2338.80444335937</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>88.782933540000002</v>
+      </c>
+      <c r="G17">
+        <v>951.46722409999995</v>
+      </c>
+      <c r="H17">
+        <v>80.466583470000003</v>
+      </c>
+      <c r="I17">
+        <v>2313.7700199999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4882,8 +5914,20 @@
       <c r="E18">
         <v>2175.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>89.847306529999997</v>
+      </c>
+      <c r="G18">
+        <v>897.05731200000002</v>
+      </c>
+      <c r="H18">
+        <v>81.444120909999995</v>
+      </c>
+      <c r="I18">
+        <v>2150.6447750000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4899,8 +5943,20 @@
       <c r="E19">
         <v>2040.57275390625</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>89.927496329999997</v>
+      </c>
+      <c r="G19">
+        <v>915.60192870000003</v>
+      </c>
+      <c r="H19">
+        <v>79.586106490000006</v>
+      </c>
+      <c r="I19">
+        <v>2374.544922</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4916,8 +5972,20 @@
       <c r="E20">
         <v>2222.322265625</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>90.728388469999999</v>
+      </c>
+      <c r="G20">
+        <v>870.22143549999998</v>
+      </c>
+      <c r="H20">
+        <v>80.983083750000006</v>
+      </c>
+      <c r="I20">
+        <v>2233.4907229999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4933,8 +6001,20 @@
       <c r="E21">
         <v>2055.74780273437</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>90.647668390000007</v>
+      </c>
+      <c r="G21">
+        <v>880.37701419999996</v>
+      </c>
+      <c r="H21">
+        <v>80.65030505</v>
+      </c>
+      <c r="I21">
+        <v>2305.0996089999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4950,8 +6030,20 @@
       <c r="E22">
         <v>2087.92211914062</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>91.001683499999999</v>
+      </c>
+      <c r="G22">
+        <v>866.34460449999995</v>
+      </c>
+      <c r="H22">
+        <v>81.468386019999997</v>
+      </c>
+      <c r="I22">
+        <v>2179.7448730000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4967,8 +6059,20 @@
       <c r="E23">
         <v>1967.65515136718</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>91.982758619999998</v>
+      </c>
+      <c r="G23">
+        <v>813.19372559999999</v>
+      </c>
+      <c r="H23">
+        <v>82.882695510000005</v>
+      </c>
+      <c r="I23">
+        <v>1968.4338379999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -4984,8 +6088,20 @@
       <c r="E24">
         <v>2076.2841796875</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>91.995192309999993</v>
+      </c>
+      <c r="G24">
+        <v>817.13684079999996</v>
+      </c>
+      <c r="H24">
+        <v>81.880892959999997</v>
+      </c>
+      <c r="I24">
+        <v>2098.0234380000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5001,8 +6117,20 @@
       <c r="E25">
         <v>1987.18139648437</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>92.386541469999997</v>
+      </c>
+      <c r="G25">
+        <v>784.27227779999998</v>
+      </c>
+      <c r="H25">
+        <v>82.182473659999999</v>
+      </c>
+      <c r="I25">
+        <v>2159.5668949999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -5018,8 +6146,20 @@
       <c r="E26">
         <v>2061.52197265625</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>92.496177369999998</v>
+      </c>
+      <c r="G26">
+        <v>782.26184079999996</v>
+      </c>
+      <c r="H26">
+        <v>82.189406539999993</v>
+      </c>
+      <c r="I26">
+        <v>2111.4914549999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -5035,8 +6175,20 @@
       <c r="E27">
         <v>1878.10717773437</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>92.795216740000001</v>
+      </c>
+      <c r="G27">
+        <v>778.23474120000003</v>
+      </c>
+      <c r="H27">
+        <v>81.953688299999996</v>
+      </c>
+      <c r="I27">
+        <v>2148.7602539999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -5052,8 +6204,20 @@
       <c r="E28">
         <v>1879.45275878906</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>92.918535129999995</v>
+      </c>
+      <c r="G28">
+        <v>756.52508539999997</v>
+      </c>
+      <c r="H28">
+        <v>83.187742650000004</v>
+      </c>
+      <c r="I28">
+        <v>2022.4293210000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5069,8 +6233,20 @@
       <c r="E29">
         <v>1875.59802246093</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>93.512705530000005</v>
+      </c>
+      <c r="G29">
+        <v>698.95031740000002</v>
+      </c>
+      <c r="H29">
+        <v>82.581114810000003</v>
+      </c>
+      <c r="I29">
+        <v>2077.8610840000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5086,8 +6262,20 @@
       <c r="E30">
         <v>1935.28686523437</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>93.744394619999994</v>
+      </c>
+      <c r="G30">
+        <v>671.10034180000002</v>
+      </c>
+      <c r="H30">
+        <v>83.569051580000007</v>
+      </c>
+      <c r="I30">
+        <v>2001.299927</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5103,8 +6291,20 @@
       <c r="E31">
         <v>1743.70593261718</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>93.7593423</v>
+      </c>
+      <c r="G31">
+        <v>662.51641849999999</v>
+      </c>
+      <c r="H31">
+        <v>82.425124789999998</v>
+      </c>
+      <c r="I31">
+        <v>2162.5109859999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5120,8 +6320,20 @@
       <c r="E32">
         <v>1955.52185058593</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>94.129297458893802</v>
+      </c>
+      <c r="G32">
+        <v>621.66497802734295</v>
+      </c>
+      <c r="H32">
+        <v>83.4061286744315</v>
+      </c>
+      <c r="I32">
+        <v>2014.80822753906</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -5137,8 +6349,20 @@
       <c r="E33">
         <v>1863.99829101562</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>94.222720478325797</v>
+      </c>
+      <c r="G33">
+        <v>599.49212646484295</v>
+      </c>
+      <c r="H33">
+        <v>83.270937326677696</v>
+      </c>
+      <c r="I33">
+        <v>2070.4775390625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -5154,8 +6378,20 @@
       <c r="E34">
         <v>1746.90612792968</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>94.155455904334801</v>
+      </c>
+      <c r="G34">
+        <v>607.22607421875</v>
+      </c>
+      <c r="H34">
+        <v>82.321131447587305</v>
+      </c>
+      <c r="I34">
+        <v>2241.36645507812</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -5171,8 +6407,20 @@
       <c r="E35">
         <v>1796.40893554687</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>94.816890881913295</v>
+      </c>
+      <c r="G35">
+        <v>547.78076171875</v>
+      </c>
+      <c r="H35">
+        <v>82.556849694952803</v>
+      </c>
+      <c r="I35">
+        <v>2177.02709960937</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -5188,8 +6436,20 @@
       <c r="E36">
         <v>1845.69934082031</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>94.783258594917697</v>
+      </c>
+      <c r="G36">
+        <v>555.03466796875</v>
+      </c>
+      <c r="H36">
+        <v>83.184276206322707</v>
+      </c>
+      <c r="I36">
+        <v>2107.146484375</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -5205,8 +6465,20 @@
       <c r="E37">
         <v>1812.06774902343</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>94.633781763826605</v>
+      </c>
+      <c r="G37">
+        <v>561.5966796875</v>
+      </c>
+      <c r="H37">
+        <v>83.901830282861894</v>
+      </c>
+      <c r="I37">
+        <v>2017.041015625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -5222,8 +6494,20 @@
       <c r="E38">
         <v>1704.71154785156</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>94.947683109118003</v>
+      </c>
+      <c r="G38">
+        <v>516.11614990234295</v>
+      </c>
+      <c r="H38">
+        <v>82.997088186355995</v>
+      </c>
+      <c r="I38">
+        <v>2129.21508789062</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -5239,8 +6523,20 @@
       <c r="E39">
         <v>1784.771484375</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>95.411061285500693</v>
+      </c>
+      <c r="G39">
+        <v>485.562255859375</v>
+      </c>
+      <c r="H39">
+        <v>83.191209095951194</v>
+      </c>
+      <c r="I39">
+        <v>2137.876953125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -5256,8 +6552,20 @@
       <c r="E40">
         <v>1854.74536132812</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>95.526905829596402</v>
+      </c>
+      <c r="G40">
+        <v>462.63967895507801</v>
+      </c>
+      <c r="H40">
+        <v>83.4303937881309</v>
+      </c>
+      <c r="I40">
+        <v>2122.11791992187</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -5273,8 +6581,20 @@
       <c r="E41">
         <v>1730.12683105468</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>95.313901345291399</v>
+      </c>
+      <c r="G41">
+        <v>484.35003662109301</v>
+      </c>
+      <c r="H41">
+        <v>83.385330005546294</v>
+      </c>
+      <c r="I41">
+        <v>2159.12158203125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -5290,8 +6610,20 @@
       <c r="E42">
         <v>1852.68737792968</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>95.642750373691996</v>
+      </c>
+      <c r="G42">
+        <v>452.96243286132801</v>
+      </c>
+      <c r="H42">
+        <v>83.641846921796997</v>
+      </c>
+      <c r="I42">
+        <v>2126.5498046875</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -5307,8 +6639,20 @@
       <c r="E43">
         <v>1819.9072265625</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>95.766068759342303</v>
+      </c>
+      <c r="G43">
+        <v>449.43307495117102</v>
+      </c>
+      <c r="H43">
+        <v>83.777038269550701</v>
+      </c>
+      <c r="I43">
+        <v>2097.83569335937</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -5324,8 +6668,20 @@
       <c r="E44">
         <v>1733.60473632812</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>95.620328849028397</v>
+      </c>
+      <c r="G44">
+        <v>457.09313964843699</v>
+      </c>
+      <c r="H44">
+        <v>83.811702717692697</v>
+      </c>
+      <c r="I44">
+        <v>2172.41015625</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -5341,8 +6697,20 @@
       <c r="E45">
         <v>1729.45935058593</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>96.079970104633702</v>
+      </c>
+      <c r="G45">
+        <v>402.15637207031199</v>
+      </c>
+      <c r="H45">
+        <v>83.985024958402605</v>
+      </c>
+      <c r="I45">
+        <v>2103.43701171875</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -5358,8 +6726,20 @@
       <c r="E46">
         <v>1798.61389160156</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>95.874439461883398</v>
+      </c>
+      <c r="G46">
+        <v>426.25921630859301</v>
+      </c>
+      <c r="H46">
+        <v>84.362867443150293</v>
+      </c>
+      <c r="I46">
+        <v>2053.2470703125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -5375,8 +6755,20 @@
       <c r="E47">
         <v>1793.21154785156</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>95.769805680119504</v>
+      </c>
+      <c r="G47">
+        <v>418.59878540039</v>
+      </c>
+      <c r="H47">
+        <v>83.704242928452501</v>
+      </c>
+      <c r="I47">
+        <v>2182.51147460937</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -5392,8 +6784,20 @@
       <c r="E48">
         <v>1709.67504882812</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>96.147234678624798</v>
+      </c>
+      <c r="G48">
+        <v>398.88113403320301</v>
+      </c>
+      <c r="H48">
+        <v>83.666112035496397</v>
+      </c>
+      <c r="I48">
+        <v>2200.10913085937</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -5409,8 +6813,20 @@
       <c r="E49">
         <v>1744.92175292968</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>96.177130044842997</v>
+      </c>
+      <c r="G49">
+        <v>387.63302612304602</v>
+      </c>
+      <c r="H49">
+        <v>84.023155851358794</v>
+      </c>
+      <c r="I49">
+        <v>2190.8212890625</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -5426,8 +6842,20 @@
       <c r="E50">
         <v>1750.38696289062</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>96.259342301943093</v>
+      </c>
+      <c r="G50">
+        <v>377.62649536132801</v>
+      </c>
+      <c r="H50">
+        <v>83.856766500277303</v>
+      </c>
+      <c r="I50">
+        <v>2133.96240234375</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -5443,8 +6871,20 @@
       <c r="E51">
         <v>1737.15539550781</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>96.296711509715905</v>
+      </c>
+      <c r="G51">
+        <v>379.46697998046801</v>
+      </c>
+      <c r="H51">
+        <v>84.758042151968894</v>
+      </c>
+      <c r="I51">
+        <v>2087.52758789062</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -5460,8 +6900,20 @@
       <c r="E52">
         <v>1777.75439453125</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>96.263079222720407</v>
+      </c>
+      <c r="G52">
+        <v>375.00848388671801</v>
+      </c>
+      <c r="H52">
+        <v>83.035219079312199</v>
+      </c>
+      <c r="I52">
+        <v>2222.9765625</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -5477,8 +6929,20 @@
       <c r="E53">
         <v>1776.37036132812</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>96.677877428998499</v>
+      </c>
+      <c r="G53">
+        <v>358.18258666992102</v>
+      </c>
+      <c r="H53">
+        <v>84.463394342762001</v>
+      </c>
+      <c r="I53">
+        <v>2095.80126953125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -5494,8 +6958,20 @@
       <c r="E54">
         <v>1783.88305664062</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>96.513452914798194</v>
+      </c>
+      <c r="G54">
+        <v>360.98452758789</v>
+      </c>
+      <c r="H54">
+        <v>83.607182473655001</v>
+      </c>
+      <c r="I54">
+        <v>2284.13208007812</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -5511,8 +6987,20 @@
       <c r="E55">
         <v>1741.46020507812</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>96.603139013452903</v>
+      </c>
+      <c r="G55">
+        <v>344.29818725585898</v>
+      </c>
+      <c r="H55">
+        <v>84.300471436494703</v>
+      </c>
+      <c r="I55">
+        <v>2185.57568359375</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -5528,8 +7016,20 @@
       <c r="E56">
         <v>1752.20031738281</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>96.6704035874439</v>
+      </c>
+      <c r="G56">
+        <v>332.98245239257801</v>
+      </c>
+      <c r="H56">
+        <v>84.737243483083702</v>
+      </c>
+      <c r="I56">
+        <v>2097.6953125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -5545,8 +7045,20 @@
       <c r="E57">
         <v>1758.38049316406</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>96.603139013452903</v>
+      </c>
+      <c r="G57">
+        <v>340.19583129882801</v>
+      </c>
+      <c r="H57">
+        <v>84.380199667221305</v>
+      </c>
+      <c r="I57">
+        <v>2132.11010742187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -5562,8 +7074,20 @@
       <c r="E58">
         <v>1732.55615234375</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>96.875934230194304</v>
+      </c>
+      <c r="G58">
+        <v>325.78228759765602</v>
+      </c>
+      <c r="H58">
+        <v>84.654048807542907</v>
+      </c>
+      <c r="I58">
+        <v>2158.64453125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -5579,8 +7103,20 @@
       <c r="E59">
         <v>1723.07360839843</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>96.860986547085204</v>
+      </c>
+      <c r="G59">
+        <v>322.43563842773398</v>
+      </c>
+      <c r="H59">
+        <v>84.258874098724306</v>
+      </c>
+      <c r="I59">
+        <v>2132.5341796875</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -5596,8 +7132,20 @@
       <c r="E60">
         <v>1803.59411621093</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>96.842301943198805</v>
+      </c>
+      <c r="G60">
+        <v>316.82492065429602</v>
+      </c>
+      <c r="H60">
+        <v>84.487659456461401</v>
+      </c>
+      <c r="I60">
+        <v>2219.94750976562</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -5613,8 +7161,20 @@
       <c r="E61">
         <v>1730.42468261718</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>97.010463378176297</v>
+      </c>
+      <c r="G61">
+        <v>318.410552978515</v>
+      </c>
+      <c r="H61">
+        <v>84.075152523571802</v>
+      </c>
+      <c r="I61">
+        <v>2244.015625</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -5630,8 +7190,20 @@
       <c r="E62">
         <v>1695.65417480468</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>96.920777279521602</v>
+      </c>
+      <c r="G62">
+        <v>319.89273071289</v>
+      </c>
+      <c r="H62">
+        <v>84.120216306156394</v>
+      </c>
+      <c r="I62">
+        <v>2258.71215820312</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -5647,8 +7219,20 @@
       <c r="E63">
         <v>1737.51794433593</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>96.875934230194304</v>
+      </c>
+      <c r="G63">
+        <v>321.06829833984301</v>
+      </c>
+      <c r="H63">
+        <v>84.383666112035499</v>
+      </c>
+      <c r="I63">
+        <v>2192.31811523437</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -5664,8 +7248,20 @@
       <c r="E64">
         <v>1761.22229003906</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>97.320627802690495</v>
+      </c>
+      <c r="G64">
+        <v>285.01052856445301</v>
+      </c>
+      <c r="H64">
+        <v>84.723377703826898</v>
+      </c>
+      <c r="I64">
+        <v>2164.91381835937</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -5681,8 +7277,20 @@
       <c r="E65">
         <v>1741.27404785156</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>97.096412556053806</v>
+      </c>
+      <c r="G65">
+        <v>292.65679931640602</v>
+      </c>
+      <c r="H65">
+        <v>84.179145867997704</v>
+      </c>
+      <c r="I65">
+        <v>2202.30493164062</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -5698,8 +7306,20 @@
       <c r="E66">
         <v>1838.77673339843</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>97.2346786248131</v>
+      </c>
+      <c r="G66">
+        <v>284.40121459960898</v>
+      </c>
+      <c r="H66">
+        <v>84.785773710482502</v>
+      </c>
+      <c r="I66">
+        <v>2146.08911132812</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -5715,8 +7335,20 @@
       <c r="E67">
         <v>1675.74536132812</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>97.275784753363197</v>
+      </c>
+      <c r="G67">
+        <v>279.76776123046801</v>
+      </c>
+      <c r="H67">
+        <v>84.543122573488603</v>
+      </c>
+      <c r="I67">
+        <v>2200.2900390625</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -5732,8 +7364,20 @@
       <c r="E68">
         <v>1673.96203613281</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>97.115097159940206</v>
+      </c>
+      <c r="G68">
+        <v>282.517822265625</v>
+      </c>
+      <c r="H68">
+        <v>83.835967831392097</v>
+      </c>
+      <c r="I68">
+        <v>2300.919921875</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -5749,8 +7393,20 @@
       <c r="E69">
         <v>1658.81616210937</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>97.320627802690495</v>
+      </c>
+      <c r="G69">
+        <v>270.57080078125</v>
+      </c>
+      <c r="H69">
+        <v>84.737243483083702</v>
+      </c>
+      <c r="I69">
+        <v>2239.9287109375</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -5766,8 +7422,20 @@
       <c r="E70">
         <v>1780.61999511718</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>97.399103139013405</v>
+      </c>
+      <c r="G70">
+        <v>270.22692871093699</v>
+      </c>
+      <c r="H70">
+        <v>84.283139212423706</v>
+      </c>
+      <c r="I70">
+        <v>2204.99658203125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -5783,8 +7451,20 @@
       <c r="E71">
         <v>1713.24035644531</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>97.305680119581396</v>
+      </c>
+      <c r="G71">
+        <v>274.60610961914</v>
+      </c>
+      <c r="H71">
+        <v>84.432196339434199</v>
+      </c>
+      <c r="I71">
+        <v>2260.31762695312</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -5800,8 +7480,20 @@
       <c r="E72">
         <v>1753.7724609375</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>97.331838565022395</v>
+      </c>
+      <c r="G72">
+        <v>269.64254760742102</v>
+      </c>
+      <c r="H72">
+        <v>84.678313921242307</v>
+      </c>
+      <c r="I72">
+        <v>2241.73999023437</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -5817,8 +7509,20 @@
       <c r="E73">
         <v>1715.64709472656</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>97.552316890881897</v>
+      </c>
+      <c r="G73">
+        <v>254.59205627441401</v>
+      </c>
+      <c r="H73">
+        <v>84.848169717138106</v>
+      </c>
+      <c r="I73">
+        <v>2228.33422851562</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -5834,8 +7538,20 @@
       <c r="E74">
         <v>1860.20227050781</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>97.212257100149401</v>
+      </c>
+      <c r="G74">
+        <v>277.28131103515602</v>
+      </c>
+      <c r="H74">
+        <v>84.206877426511298</v>
+      </c>
+      <c r="I74">
+        <v>2281.2568359375</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -5851,8 +7567,20 @@
       <c r="E75">
         <v>1819.66564941406</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>97.690582959641205</v>
+      </c>
+      <c r="G75">
+        <v>241.49928283691401</v>
+      </c>
+      <c r="H75">
+        <v>84.657515252357101</v>
+      </c>
+      <c r="I75">
+        <v>2295.232421875</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -5868,8 +7596,20 @@
       <c r="E76">
         <v>1791.12316894531</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>97.612107623318394</v>
+      </c>
+      <c r="G76">
+        <v>234.65965270996</v>
+      </c>
+      <c r="H76">
+        <v>84.491125901275595</v>
+      </c>
+      <c r="I76">
+        <v>2313.78247070312</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -5885,8 +7625,20 @@
       <c r="E77">
         <v>1800.41650390625</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <v>97.623318385650194</v>
+      </c>
+      <c r="G77">
+        <v>243.79116821289</v>
+      </c>
+      <c r="H77">
+        <v>84.154880754298304</v>
+      </c>
+      <c r="I77">
+        <v>2349.74487304687</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -5902,8 +7654,20 @@
       <c r="E78">
         <v>1732.12084960937</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <v>97.634529147981993</v>
+      </c>
+      <c r="G78">
+        <v>235.63536071777301</v>
+      </c>
+      <c r="H78">
+        <v>85.132418191902303</v>
+      </c>
+      <c r="I78">
+        <v>2228.49487304687</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -5919,8 +7683,20 @@
       <c r="E79">
         <v>1885.6181640625</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>97.619581464872894</v>
+      </c>
+      <c r="G79">
+        <v>250.30729675292901</v>
+      </c>
+      <c r="H79">
+        <v>84.168746533555094</v>
+      </c>
+      <c r="I79">
+        <v>2352.32397460937</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -5936,8 +7712,20 @@
       <c r="E80">
         <v>1889.95471191406</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <v>97.713004484304903</v>
+      </c>
+      <c r="G80">
+        <v>237.21122741699199</v>
+      </c>
+      <c r="H80">
+        <v>84.719911259012704</v>
+      </c>
+      <c r="I80">
+        <v>2246.421875</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -5953,8 +7741,20 @@
       <c r="E81">
         <v>1839.31750488281</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <v>97.675635276532105</v>
+      </c>
+      <c r="G81">
+        <v>239.29904174804599</v>
+      </c>
+      <c r="H81">
+        <v>84.470327232390403</v>
+      </c>
+      <c r="I81">
+        <v>2419.63891601562</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -5970,8 +7770,20 @@
       <c r="E82">
         <v>1799.03112792968</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>97.754110612855001</v>
+      </c>
+      <c r="G82">
+        <v>232.43489074707</v>
+      </c>
+      <c r="H82">
+        <v>84.622850804215204</v>
+      </c>
+      <c r="I82">
+        <v>2315.99145507812</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -5987,8 +7799,20 @@
       <c r="E83">
         <v>1846.53137207031</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <v>97.832585949177798</v>
+      </c>
+      <c r="G83">
+        <v>215.68127441406199</v>
+      </c>
+      <c r="H83">
+        <v>85.011092623405403</v>
+      </c>
+      <c r="I83">
+        <v>2316.21166992187</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -6004,8 +7828,20 @@
       <c r="E84">
         <v>1866.04541015625</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <v>97.776532137518601</v>
+      </c>
+      <c r="G84">
+        <v>228.06394958496</v>
+      </c>
+      <c r="H84">
+        <v>84.910565723793596</v>
+      </c>
+      <c r="I84">
+        <v>2281.05859375</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -6021,8 +7857,20 @@
       <c r="E85">
         <v>1731.16674804687</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <v>97.862481315396096</v>
+      </c>
+      <c r="G85">
+        <v>214.60850524902301</v>
+      </c>
+      <c r="H85">
+        <v>84.771907931225698</v>
+      </c>
+      <c r="I85">
+        <v>2259.4287109375</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -6038,8 +7886,20 @@
       <c r="E86">
         <v>1773.14733886718</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <v>97.713004484304903</v>
+      </c>
+      <c r="G86">
+        <v>225.80044555664</v>
+      </c>
+      <c r="H86">
+        <v>84.570854132002196</v>
+      </c>
+      <c r="I86">
+        <v>2345.05029296875</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -6055,8 +7915,20 @@
       <c r="E87">
         <v>1861.85485839843</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <v>97.813901345291399</v>
+      </c>
+      <c r="G87">
+        <v>225.41110229492099</v>
+      </c>
+      <c r="H87">
+        <v>84.078618968385996</v>
+      </c>
+      <c r="I87">
+        <v>2380.4287109375</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -6072,8 +7944,20 @@
       <c r="E88">
         <v>1701.42639160156</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88">
+        <v>97.769058295964101</v>
+      </c>
+      <c r="G88">
+        <v>226.17283630371</v>
+      </c>
+      <c r="H88">
+        <v>84.751109262340506</v>
+      </c>
+      <c r="I88">
+        <v>2321.81274414062</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -6089,8 +7973,20 @@
       <c r="E89">
         <v>1839.04553222656</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <v>98.090433482810099</v>
+      </c>
+      <c r="G89">
+        <v>203.05740356445301</v>
+      </c>
+      <c r="H89">
+        <v>84.6817803660565</v>
+      </c>
+      <c r="I89">
+        <v>2342.87524414062</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -6106,8 +8002,20 @@
       <c r="E90">
         <v>1911.90991210937</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90">
+        <v>98.015695067264502</v>
+      </c>
+      <c r="G90">
+        <v>195.89602661132801</v>
+      </c>
+      <c r="H90">
+        <v>84.841236827509704</v>
+      </c>
+      <c r="I90">
+        <v>2310.34594726562</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -6123,8 +8031,20 @@
       <c r="E91">
         <v>1846.60925292968</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91">
+        <v>97.754110612855001</v>
+      </c>
+      <c r="G91">
+        <v>220.155014038085</v>
+      </c>
+      <c r="H91">
+        <v>84.130615640599004</v>
+      </c>
+      <c r="I91">
+        <v>2487.59252929687</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -6140,8 +8060,20 @@
       <c r="E92">
         <v>1808.556640625</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92">
+        <v>98.041853512705501</v>
+      </c>
+      <c r="G92">
+        <v>204.89091491699199</v>
+      </c>
+      <c r="H92">
+        <v>84.657515252357101</v>
+      </c>
+      <c r="I92">
+        <v>2351.63696289062</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -6157,8 +8089,20 @@
       <c r="E93">
         <v>1719.55139160156</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93">
+        <v>97.836322869955097</v>
+      </c>
+      <c r="G93">
+        <v>226.47520446777301</v>
+      </c>
+      <c r="H93">
+        <v>84.751109262340506</v>
+      </c>
+      <c r="I93">
+        <v>2333.14404296875</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -6174,8 +8118,20 @@
       <c r="E94">
         <v>1878.27087402343</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94">
+        <v>98.049327354260001</v>
+      </c>
+      <c r="G94">
+        <v>200.84881591796801</v>
+      </c>
+      <c r="H94">
+        <v>84.813505268996096</v>
+      </c>
+      <c r="I94">
+        <v>2330.47387695312</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -6191,8 +8147,20 @@
       <c r="E95">
         <v>1777.29162597656</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <v>97.888639760836995</v>
+      </c>
+      <c r="G95">
+        <v>212.31690979003901</v>
+      </c>
+      <c r="H95">
+        <v>84.355934553521905</v>
+      </c>
+      <c r="I95">
+        <v>2412.3115234375</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -6208,8 +8176,20 @@
       <c r="E96">
         <v>1812.73120117187</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96">
+        <v>98.127802690582897</v>
+      </c>
+      <c r="G96">
+        <v>187.22636413574199</v>
+      </c>
+      <c r="H96">
+        <v>85.461730449251206</v>
+      </c>
+      <c r="I96">
+        <v>2258.31420898437</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -6225,8 +8205,20 @@
       <c r="E97">
         <v>1834.84069824218</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97">
+        <v>98.011958146487302</v>
+      </c>
+      <c r="G97">
+        <v>196.883056640625</v>
+      </c>
+      <c r="H97">
+        <v>84.269273433166902</v>
+      </c>
+      <c r="I97">
+        <v>2458.80029296875</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -6242,8 +8234,20 @@
       <c r="E98">
         <v>1885.92248535156</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98">
+        <v>98.127802690582897</v>
+      </c>
+      <c r="G98">
+        <v>188.84878540039</v>
+      </c>
+      <c r="H98">
+        <v>84.7060454797559</v>
+      </c>
+      <c r="I98">
+        <v>2329.93603515625</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -6259,8 +8263,20 @@
       <c r="E99">
         <v>1821.76635742187</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99">
+        <v>97.963378176382605</v>
+      </c>
+      <c r="G99">
+        <v>198.51150512695301</v>
+      </c>
+      <c r="H99">
+        <v>84.394065446478095</v>
+      </c>
+      <c r="I99">
+        <v>2386.41918945312</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -6276,8 +8292,20 @@
       <c r="E100">
         <v>1791.43676757812</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100">
+        <v>98.307174887892302</v>
+      </c>
+      <c r="G100">
+        <v>179.83720397949199</v>
+      </c>
+      <c r="H100">
+        <v>84.789240155296696</v>
+      </c>
+      <c r="I100">
+        <v>2407.47583007812</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -6292,6 +8320,18 @@
       </c>
       <c r="E101">
         <v>1864.82666015625</v>
+      </c>
+      <c r="F101">
+        <v>98.120328849028397</v>
+      </c>
+      <c r="G101">
+        <v>182.00682067871</v>
+      </c>
+      <c r="H101">
+        <v>84.473793677204597</v>
+      </c>
+      <c r="I101">
+        <v>2493.00463867187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>